<commit_message>
Updated Monte Carlo simulations, added export functions
</commit_message>
<xml_diff>
--- a/dataset_examples/dataset.xlsx
+++ b/dataset_examples/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbrac\OneDrive\Área de Trabalho\dietcost_brasileiro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbrac\OneDrive\Documentos\Nutrição\Produtos\Pacote\dietcost\dataset_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D0A5A3-F226-4C5D-9EB4-A6160EA94554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAE9064-A2CF-42C4-AAAD-33410FBBC7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{666473FE-F6BD-40E0-A450-02D420181B78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="10" xr2:uid="{666473FE-F6BD-40E0-A450-02D420181B78}"/>
   </bookViews>
   <sheets>
     <sheet name="nutrient_targets" sheetId="11" r:id="rId1"/>
@@ -974,6 +974,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44119D87-2AAD-4080-8CB0-D31119E3C8C4}" name="Tabela1" displayName="Tabela1" ref="A1:J100" totalsRowShown="0">
+  <autoFilter ref="A1:J100" xr:uid="{44119D87-2AAD-4080-8CB0-D31119E3C8C4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J100">
+    <sortCondition ref="B1:B100"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{7BCD878C-3640-4429-9B7B-221BA57B4AA1}" name="food_name"/>
+    <tableColumn id="2" xr3:uid="{89875A0F-62E9-443F-86E9-7A9A45BB9800}" name="food_id"/>
+    <tableColumn id="3" xr3:uid="{8069D27E-CF6C-4A45-A5B1-7D8CC0A774BB}" name="energy_kj_g"/>
+    <tableColumn id="4" xr3:uid="{B219E1F2-6DED-4770-ADBE-D40021C5E503}" name="fat_g"/>
+    <tableColumn id="5" xr3:uid="{F82AC198-7440-41B1-83AE-9C6A5B9359F6}" name="sat_fat_g"/>
+    <tableColumn id="6" xr3:uid="{AD784DB8-D8E7-4B99-BA7E-7D19F19A4943}" name="CHO_g"/>
+    <tableColumn id="7" xr3:uid="{B25B91AD-07AA-45B0-8220-D1AFDCA0C5DB}" name="sugars_g"/>
+    <tableColumn id="8" xr3:uid="{E59560D9-541A-49BB-BF91-63F6645E7527}" name="fibre_g"/>
+    <tableColumn id="9" xr3:uid="{61ECE55B-A0CE-4A1D-8699-7E2BD96A8ABD}" name="protein_g"/>
+    <tableColumn id="10" xr3:uid="{680F7FA2-4DE0-4DD2-BB9F-C52B5AA69E6D}" name="sodium_mg"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3934,11 +3956,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAA402D-1497-4FF1-AFAA-03484A88CC1C}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7142,6 +7175,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -18699,7 +18735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3AC532-FA6B-4276-8595-9C2C1483DB0A}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>